<commit_message>
Add NIST CSF and CIS support
</commit_message>
<xml_diff>
--- a/results/ISO_2022 Result Sheet Government Sector 2021-2023.xlsx
+++ b/results/ISO_2022 Result Sheet Government Sector 2021-2023.xlsx
@@ -17,15 +17,15 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12117" uniqueCount="1541">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12117" uniqueCount="1595">
+  <si>
+    <t>ttp_weight</t>
+  </si>
+  <si>
+    <t>Control ID</t>
+  </si>
   <si>
     <t>Control Name</t>
-  </si>
-  <si>
-    <t>ttp_weight</t>
-  </si>
-  <si>
-    <t>Control ID</t>
   </si>
   <si>
     <t>Management of technical vulnerabilities</t>
@@ -4714,7 +4714,169 @@
     <t>['Information theft and espionage', 'Financial gain']</t>
   </si>
   <si>
-    <t>Government</t>
+    <t>['Defense', 'Financial', 'Government', 'Healthcare', 'Telecommunications']</t>
+  </si>
+  <si>
+    <t>['Aerospace', 'Defense', 'Energy', 'Engineering', 'Financial', 'Government', 'Healthcare', 'Media', 'Shipping and Logistics', 'Technology']</t>
+  </si>
+  <si>
+    <t>['Defense', 'Government', 'Law enforcement', 'NGOs']</t>
+  </si>
+  <si>
+    <t>['Defense', 'Energy', 'Financial', 'Government', 'Healthcare', 'Manufacturing', 'Retail', 'Shipping and Logistics', 'Utilities', 'Technology']</t>
+  </si>
+  <si>
+    <t>['Defense', 'Education', 'Government', 'Media']</t>
+  </si>
+  <si>
+    <t>['Aerospace', 'Defense', 'Education', 'Energy', 'Financial', 'Government', 'Healthcare', 'Law enforcement', 'Media', 'NGOs', 'Pharmaceutical', 'Telecommunications', 'Transportation', 'Think Tanks']</t>
+  </si>
+  <si>
+    <t>['Defense', 'Energy', 'Financial', 'Government', 'Healthcare', 'IT', 'Oil and gas', 'Technology', 'Telecommunications']</t>
+  </si>
+  <si>
+    <t>['Aerospace', 'Automotive', 'Chemical', 'Financial', 'Government', 'Healthcare', 'High-Tech', 'Manufacturing', 'Technology', 'Transportation']</t>
+  </si>
+  <si>
+    <t>['Energy', 'Financial', 'Government', 'Media', 'Transportation']</t>
+  </si>
+  <si>
+    <t>['Defense', 'Education', 'Energy', 'Government', 'Healthcare', 'Think Tanks']</t>
+  </si>
+  <si>
+    <t>['Aviation', 'Education', 'Government', 'NGOs', 'Think Tanks', 'Telecommunications']</t>
+  </si>
+  <si>
+    <t>['Education', 'Energy', 'Government', 'Telecommunications']</t>
+  </si>
+  <si>
+    <t>['Government', 'Manufacturing']</t>
+  </si>
+  <si>
+    <t>['Construction', 'Defense', 'Education', 'Energy', 'Financial', 'Government', 'Healthcare', 'High-Tech', 'Hospitality', 'Manufacturing', 'Media', 'Oil and gas', 'Petrochemical', 'Pharmaceutical', 'Retail', 'Telecommunications', 'Transportation', 'Online video game companies']</t>
+  </si>
+  <si>
+    <t>['Automotive', 'Aviation', 'Chemical', 'Construction', 'Defense', 'Education', 'Embassies', 'Engineering', 'Financial', 'Government', 'Healthcare', 'Industrial', 'IT', 'Media', 'NGOs', 'Oil and gas', 'Think Tanks']</t>
+  </si>
+  <si>
+    <t>['Aviation', 'Chemical', 'Education', 'Energy', 'Financial', 'Government', 'High-Tech', 'Hospitality', 'Oil and gas', 'Telecommunications']</t>
+  </si>
+  <si>
+    <t>['Aerospace', 'Aviation', 'Defense', 'Education', 'Embassies', 'Government', 'Manufacturing', 'Technology', 'Telecommunications', 'Think Tanks']</t>
+  </si>
+  <si>
+    <t>['Defense', 'Embassies', 'Government']</t>
+  </si>
+  <si>
+    <t>['Aerospace', 'Defense', 'Education', 'Embassies', 'Energy', 'Government', 'High-Tech', 'IT', 'Media', 'NGOs', 'Pharmaceutical', 'Research', 'Retail']</t>
+  </si>
+  <si>
+    <t>['Financial', 'Government', 'Healthcare', 'Media']</t>
+  </si>
+  <si>
+    <t>['Defense', 'Education', 'Energy', 'Financial', 'Food and Agriculture', 'Gaming', 'Government', 'Healthcare', 'High-Tech', 'IT', 'Media', 'NGOs', 'Oil and gas', 'Telecommunications', 'Transportation']</t>
+  </si>
+  <si>
+    <t>['Construction', 'Education', 'Energy', 'Financial', 'Government', 'Healthcare', 'Hospitality', 'IT', 'Manufacturing', 'Media', 'Non-profit organizations', 'Oil and gas', 'Retail', 'Shipping and Logistics', 'Technology', 'Telecommunications', 'Transportation']</t>
+  </si>
+  <si>
+    <t>['Energy', 'Engineering', 'Government']</t>
+  </si>
+  <si>
+    <t>['Government', 'Law enforcement', 'Telecommunications']</t>
+  </si>
+  <si>
+    <t>['Defense', 'Government']</t>
+  </si>
+  <si>
+    <t>['Financial', 'Government']</t>
+  </si>
+  <si>
+    <t>['Energy', 'Financial', 'Government', 'Healthcare', 'Manufacturing']</t>
+  </si>
+  <si>
+    <t>['Casinos and Gambling', 'Construction', 'Education', 'Energy', 'Financial', 'Government', 'High-Tech', 'Hospitality', 'Retail', 'Technology', 'Telecommunications', 'Transportation']</t>
+  </si>
+  <si>
+    <t>['Energy', 'Financial', 'Government', 'Manufacturing', 'Transportation', 'Utilities']</t>
+  </si>
+  <si>
+    <t>['Aerospace', 'Defense', 'Embassies', 'Energy', 'Financial', 'Government', 'High-Tech', 'Media', 'Oil and gas', 'Telecommunications']</t>
+  </si>
+  <si>
+    <t>['Aerospace', 'Defense', 'Energy', 'Financial', 'Government', 'Healthcare', 'High-Tech', 'IT', 'Media', 'NGOs', 'Pharmaceutical', 'Telecommunications']</t>
+  </si>
+  <si>
+    <t>['Government']</t>
+  </si>
+  <si>
+    <t>['Financial', 'Government', 'Telecommunications']</t>
+  </si>
+  <si>
+    <t>['Automotive', 'Education', 'Government', 'Healthcare', 'Hospitality', 'Manufacturing', 'Media', 'Retail', 'Technology']</t>
+  </si>
+  <si>
+    <t>['Aerospace', 'Aviation', 'Chemical', 'Defense', 'Embassies', 'Energy', 'Government', 'High-Tech', 'Industrial', 'Manufacturing', 'Mining', 'Oil and gas', 'Telecommunications', 'Utilities']</t>
+  </si>
+  <si>
+    <t>['Defense', 'Financial', 'Government', 'IT', 'Media']</t>
+  </si>
+  <si>
+    <t>['Embassies', 'Defense', 'Government']</t>
+  </si>
+  <si>
+    <t>['Financial', 'Government', 'Manufacturing', 'Pharmaceutical']</t>
+  </si>
+  <si>
+    <t>['Education', 'Government', 'Healthcare', 'Manufacturing', 'Media', 'Non-profit organizations', 'Pharmaceutical']</t>
+  </si>
+  <si>
+    <t>['Education', 'Gaming', 'Government', 'High-Tech', 'NGOs']</t>
+  </si>
+  <si>
+    <t>['Defense', 'Education', 'Energy', 'Financial', 'Government', 'High-Tech', 'Manufacturing', 'Pharmaceutical', 'Telecommunications', 'Think Tanks']</t>
+  </si>
+  <si>
+    <t>['Aerospace', 'Defense', 'Education', 'Government', 'High-Tech', 'Satellites', 'Telecommunications']</t>
+  </si>
+  <si>
+    <t>['Aerospace', 'Defense', 'Embassies', 'Energy', 'Engineering', 'Financial', 'Government', 'Oil and gas', 'Research']</t>
+  </si>
+  <si>
+    <t>['Critical infrastructure', 'Defense', 'Education', 'Government', 'Media', 'Transportation']</t>
+  </si>
+  <si>
+    <t>['Defense', 'Energy', 'Government', 'Law enforcement', 'Media']</t>
+  </si>
+  <si>
+    <t>['Defense', 'Education', 'Embassies', 'Energy', 'Government', 'Telecommunications']</t>
+  </si>
+  <si>
+    <t>['Defense', 'Energy', 'Government', 'Healthcare', 'Hospitality', 'NGOs', 'Pharmaceutical', 'Research', 'Technology']</t>
+  </si>
+  <si>
+    <t>['Defense', 'Government', 'Oil and gas', 'Telecommunications']</t>
+  </si>
+  <si>
+    <t>['Defense', 'Financial', 'Government']</t>
+  </si>
+  <si>
+    <t>['Government', 'Healthcare']</t>
+  </si>
+  <si>
+    <t>['Defense', 'Government', 'Telecommunications']</t>
+  </si>
+  <si>
+    <t>['Aviation', 'Defense', 'Energy', 'Financial', 'Government', 'IT', 'Media', 'NGOs', 'Pharmaceutical', 'Think Tanks']</t>
+  </si>
+  <si>
+    <t>['Critical infrastructure', 'Defense', 'Engineering', 'Government', 'High-Tech', 'Industrial', 'Manufacturing', 'Media', 'Technology']</t>
+  </si>
+  <si>
+    <t>['Online video game companies', 'Aviation', 'Defense', 'Education', 'Financial', 'Government', 'Healthcare', 'Pharmaceutical', 'Technology', 'Telecommunications']</t>
+  </si>
+  <si>
+    <t>['Construction', 'Energy', 'Government', 'IT', 'Manufacturing', 'Shipping and Logistics', 'Technology', 'Transportation']</t>
   </si>
   <si>
     <t>['Australia', 'Bangladesh', 'Belgium', 'Brazil', 'Canada', 'Chile', 'China', 'Ecuador', 'France', 'Germany', 'Guatemala', 'Hong Kong', 'India', 'Israel', 'Japan', 'Mexico', 'Netherlands', 'Philippines', 'Poland', 'Russia', 'South Africa', 'South Korea', 'Taiwan', 'Thailand', 'UK', 'USA', 'Vietnam']</t>
@@ -5315,20 +5477,20 @@
   <sheetData>
     <row r="1" spans="1:3">
       <c r="A1" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="B1" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="B1" s="1" t="s">
+      <c r="C1" s="1" t="s">
         <v>0</v>
-      </c>
-      <c r="C1" s="1" t="s">
-        <v>1</v>
       </c>
     </row>
     <row r="2" spans="1:3">
       <c r="A2" s="1">
         <v>8.800000000000001</v>
       </c>
-      <c r="B2" t="s">
+      <c r="B2" s="1" t="s">
         <v>3</v>
       </c>
       <c r="C2">
@@ -5339,7 +5501,7 @@
       <c r="A3" s="1">
         <v>8.9</v>
       </c>
-      <c r="B3" t="s">
+      <c r="B3" s="1" t="s">
         <v>4</v>
       </c>
       <c r="C3">
@@ -5350,7 +5512,7 @@
       <c r="A4" s="1">
         <v>8.1</v>
       </c>
-      <c r="B4" t="s">
+      <c r="B4" s="1" t="s">
         <v>5</v>
       </c>
       <c r="C4">
@@ -5361,7 +5523,7 @@
       <c r="A5" s="1">
         <v>8.699999999999999</v>
       </c>
-      <c r="B5" t="s">
+      <c r="B5" s="1" t="s">
         <v>6</v>
       </c>
       <c r="C5">
@@ -5372,7 +5534,7 @@
       <c r="A6" s="1">
         <v>8.199999999999999</v>
       </c>
-      <c r="B6" t="s">
+      <c r="B6" s="1" t="s">
         <v>7</v>
       </c>
       <c r="C6">
@@ -5383,7 +5545,7 @@
       <c r="A7" s="1">
         <v>8.5</v>
       </c>
-      <c r="B7" t="s">
+      <c r="B7" s="1" t="s">
         <v>8</v>
       </c>
       <c r="C7">
@@ -5394,7 +5556,7 @@
       <c r="A8" s="1">
         <v>5.15</v>
       </c>
-      <c r="B8" t="s">
+      <c r="B8" s="1" t="s">
         <v>9</v>
       </c>
       <c r="C8">
@@ -5405,7 +5567,7 @@
       <c r="A9" s="1">
         <v>8.300000000000001</v>
       </c>
-      <c r="B9" t="s">
+      <c r="B9" s="1" t="s">
         <v>10</v>
       </c>
       <c r="C9">
@@ -5416,7 +5578,7 @@
       <c r="A10" s="1">
         <v>5.18</v>
       </c>
-      <c r="B10" t="s">
+      <c r="B10" s="1" t="s">
         <v>11</v>
       </c>
       <c r="C10">
@@ -5427,7 +5589,7 @@
       <c r="A11" s="1">
         <v>6.5</v>
       </c>
-      <c r="B11" t="s">
+      <c r="B11" s="1" t="s">
         <v>12</v>
       </c>
       <c r="C11">
@@ -5438,7 +5600,7 @@
       <c r="A12" s="1">
         <v>5.16</v>
       </c>
-      <c r="B12" t="s">
+      <c r="B12" s="1" t="s">
         <v>13</v>
       </c>
       <c r="C12">
@@ -5449,7 +5611,7 @@
       <c r="A13" s="1">
         <v>5.3</v>
       </c>
-      <c r="B13" t="s">
+      <c r="B13" s="1" t="s">
         <v>14</v>
       </c>
       <c r="C13">
@@ -5460,7 +5622,7 @@
       <c r="A14" s="1">
         <v>8.16</v>
       </c>
-      <c r="B14" t="s">
+      <c r="B14" s="1" t="s">
         <v>15</v>
       </c>
       <c r="C14">
@@ -5471,7 +5633,7 @@
       <c r="A15" s="1">
         <v>8.19</v>
       </c>
-      <c r="B15" t="s">
+      <c r="B15" s="1" t="s">
         <v>16</v>
       </c>
       <c r="C15">
@@ -5482,7 +5644,7 @@
       <c r="A16" s="1">
         <v>8.210000000000001</v>
       </c>
-      <c r="B16" t="s">
+      <c r="B16" s="1" t="s">
         <v>17</v>
       </c>
       <c r="C16">
@@ -5493,7 +5655,7 @@
       <c r="A17" s="1">
         <v>8.4</v>
       </c>
-      <c r="B17" t="s">
+      <c r="B17" s="1" t="s">
         <v>18</v>
       </c>
       <c r="C17">
@@ -5504,7 +5666,7 @@
       <c r="A18" s="1">
         <v>8.27</v>
       </c>
-      <c r="B18" t="s">
+      <c r="B18" s="1" t="s">
         <v>19</v>
       </c>
       <c r="C18">
@@ -5515,7 +5677,7 @@
       <c r="A19" s="1">
         <v>8.220000000000001</v>
       </c>
-      <c r="B19" t="s">
+      <c r="B19" s="1" t="s">
         <v>20</v>
       </c>
       <c r="C19">
@@ -5526,7 +5688,7 @@
       <c r="A20" s="1">
         <v>8.23</v>
       </c>
-      <c r="B20" t="s">
+      <c r="B20" s="1" t="s">
         <v>21</v>
       </c>
       <c r="C20">
@@ -5537,7 +5699,7 @@
       <c r="A21" s="1">
         <v>6.3</v>
       </c>
-      <c r="B21" t="s">
+      <c r="B21" s="1" t="s">
         <v>22</v>
       </c>
       <c r="C21">
@@ -5548,7 +5710,7 @@
       <c r="A22" s="1">
         <v>8.279999999999999</v>
       </c>
-      <c r="B22" t="s">
+      <c r="B22" s="1" t="s">
         <v>23</v>
       </c>
       <c r="C22">
@@ -5559,7 +5721,7 @@
       <c r="A23" s="1">
         <v>8.25</v>
       </c>
-      <c r="B23" t="s">
+      <c r="B23" s="1" t="s">
         <v>24</v>
       </c>
       <c r="C23">
@@ -5570,7 +5732,7 @@
       <c r="A24" s="1">
         <v>5.8</v>
       </c>
-      <c r="B24" t="s">
+      <c r="B24" s="1" t="s">
         <v>25</v>
       </c>
       <c r="C24">
@@ -5581,7 +5743,7 @@
       <c r="A25" s="1">
         <v>6.7</v>
       </c>
-      <c r="B25" t="s">
+      <c r="B25" s="1" t="s">
         <v>26</v>
       </c>
       <c r="C25">
@@ -5592,7 +5754,7 @@
       <c r="A26" s="1">
         <v>5.17</v>
       </c>
-      <c r="B26" t="s">
+      <c r="B26" s="1" t="s">
         <v>27</v>
       </c>
       <c r="C26">
@@ -5603,7 +5765,7 @@
       <c r="A27" s="1">
         <v>5.1</v>
       </c>
-      <c r="B27" t="s">
+      <c r="B27" s="1" t="s">
         <v>28</v>
       </c>
       <c r="C27">
@@ -5614,7 +5776,7 @@
       <c r="A28" s="1">
         <v>6.8</v>
       </c>
-      <c r="B28" t="s">
+      <c r="B28" s="1" t="s">
         <v>29</v>
       </c>
       <c r="C28">
@@ -5625,7 +5787,7 @@
       <c r="A29" s="1">
         <v>8.199999999999999</v>
       </c>
-      <c r="B29" t="s">
+      <c r="B29" s="1" t="s">
         <v>30</v>
       </c>
       <c r="C29">
@@ -5636,7 +5798,7 @@
       <c r="A30" s="1">
         <v>5.9</v>
       </c>
-      <c r="B30" t="s">
+      <c r="B30" s="1" t="s">
         <v>31</v>
       </c>
       <c r="C30">
@@ -5647,7 +5809,7 @@
       <c r="A31" s="1">
         <v>8.18</v>
       </c>
-      <c r="B31" t="s">
+      <c r="B31" s="1" t="s">
         <v>32</v>
       </c>
       <c r="C31">
@@ -5658,7 +5820,7 @@
       <c r="A32" s="1">
         <v>8.31</v>
       </c>
-      <c r="B32" t="s">
+      <c r="B32" s="1" t="s">
         <v>33</v>
       </c>
       <c r="C32">
@@ -5669,7 +5831,7 @@
       <c r="A33" s="1">
         <v>8.130000000000001</v>
       </c>
-      <c r="B33" t="s">
+      <c r="B33" s="1" t="s">
         <v>34</v>
       </c>
       <c r="C33">
@@ -5680,7 +5842,7 @@
       <c r="A34" s="1">
         <v>8.15</v>
       </c>
-      <c r="B34" t="s">
+      <c r="B34" s="1" t="s">
         <v>35</v>
       </c>
       <c r="C34">
@@ -5691,7 +5853,7 @@
       <c r="A35" s="1">
         <v>8.119999999999999</v>
       </c>
-      <c r="B35" t="s">
+      <c r="B35" s="1" t="s">
         <v>36</v>
       </c>
       <c r="C35">
@@ -5702,7 +5864,7 @@
       <c r="A36" s="1">
         <v>5.14</v>
       </c>
-      <c r="B36" t="s">
+      <c r="B36" s="1" t="s">
         <v>37</v>
       </c>
       <c r="C36">
@@ -5713,7 +5875,7 @@
       <c r="A37" s="1">
         <v>8.6</v>
       </c>
-      <c r="B37" t="s">
+      <c r="B37" s="1" t="s">
         <v>38</v>
       </c>
       <c r="C37">
@@ -5724,7 +5886,7 @@
       <c r="A38" s="1">
         <v>8.289999999999999</v>
       </c>
-      <c r="B38" t="s">
+      <c r="B38" s="1" t="s">
         <v>39</v>
       </c>
       <c r="C38">
@@ -5735,7 +5897,7 @@
       <c r="A39" s="1">
         <v>5.33</v>
       </c>
-      <c r="B39" t="s">
+      <c r="B39" s="1" t="s">
         <v>40</v>
       </c>
       <c r="C39">
@@ -5746,7 +5908,7 @@
       <c r="A40" s="1">
         <v>5.1</v>
       </c>
-      <c r="B40" t="s">
+      <c r="B40" s="1" t="s">
         <v>41</v>
       </c>
       <c r="C40">
@@ -5757,7 +5919,7 @@
       <c r="A41" s="1">
         <v>5.28</v>
       </c>
-      <c r="B41" t="s">
+      <c r="B41" s="1" t="s">
         <v>42</v>
       </c>
       <c r="C41">
@@ -5768,7 +5930,7 @@
       <c r="A42" s="1">
         <v>7.1</v>
       </c>
-      <c r="B42" t="s">
+      <c r="B42" s="1" t="s">
         <v>43</v>
       </c>
       <c r="C42">
@@ -5779,7 +5941,7 @@
       <c r="A43" s="1">
         <v>5.2</v>
       </c>
-      <c r="B43" t="s">
+      <c r="B43" s="1" t="s">
         <v>44</v>
       </c>
       <c r="C43">
@@ -5790,7 +5952,7 @@
       <c r="A44" s="1">
         <v>5.19</v>
       </c>
-      <c r="B44" t="s">
+      <c r="B44" s="1" t="s">
         <v>45</v>
       </c>
       <c r="C44">
@@ -5801,7 +5963,7 @@
       <c r="A45" s="1">
         <v>8.26</v>
       </c>
-      <c r="B45" t="s">
+      <c r="B45" s="1" t="s">
         <v>46</v>
       </c>
       <c r="C45">
@@ -5812,7 +5974,7 @@
       <c r="A46" s="1">
         <v>8.300000000000001</v>
       </c>
-      <c r="B46" t="s">
+      <c r="B46" s="1" t="s">
         <v>47</v>
       </c>
       <c r="C46">
@@ -5823,7 +5985,7 @@
       <c r="A47" s="1">
         <v>7.1</v>
       </c>
-      <c r="B47" t="s">
+      <c r="B47" s="1" t="s">
         <v>48</v>
       </c>
       <c r="C47">
@@ -5845,13 +6007,13 @@
   <sheetData>
     <row r="1" spans="1:8">
       <c r="A1" s="1" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="B1" s="1" t="s">
         <v>49</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="D1" s="1" t="s">
         <v>50</v>
@@ -5866,7 +6028,7 @@
         <v>53</v>
       </c>
       <c r="H1" s="1" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="2" spans="1:8">
@@ -49449,7 +49611,7 @@
         <v>53</v>
       </c>
       <c r="F1" s="1" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="2" spans="1:6">
@@ -55865,7 +56027,7 @@
         <v>1449</v>
       </c>
       <c r="G2" t="s">
-        <v>1522</v>
+        <v>1576</v>
       </c>
       <c r="H2">
         <v>0.3162277660168379</v>
@@ -55894,13 +56056,13 @@
         <v>1458</v>
       </c>
       <c r="E3" t="s">
-        <v>1466</v>
+        <v>1467</v>
       </c>
       <c r="F3" t="s">
-        <v>1467</v>
+        <v>1521</v>
       </c>
       <c r="G3" t="s">
-        <v>1523</v>
+        <v>1577</v>
       </c>
       <c r="H3">
         <v>0.242535625036333</v>
@@ -55929,13 +56091,13 @@
         <v>1459</v>
       </c>
       <c r="E4" t="s">
-        <v>1466</v>
+        <v>1468</v>
       </c>
       <c r="F4" t="s">
-        <v>1468</v>
+        <v>1522</v>
       </c>
       <c r="G4" t="s">
-        <v>1524</v>
+        <v>1578</v>
       </c>
       <c r="H4">
         <v>0.3015113445777636</v>
@@ -55964,13 +56126,13 @@
         <v>1460</v>
       </c>
       <c r="E5" t="s">
-        <v>1466</v>
+        <v>1469</v>
       </c>
       <c r="F5" t="s">
         <v>1449</v>
       </c>
       <c r="G5" t="s">
-        <v>1522</v>
+        <v>1576</v>
       </c>
       <c r="H5">
         <v>0.3162277660168379</v>
@@ -55999,13 +56161,13 @@
         <v>1461</v>
       </c>
       <c r="E6" t="s">
-        <v>1466</v>
+        <v>1470</v>
       </c>
       <c r="F6" t="s">
-        <v>1469</v>
+        <v>1523</v>
       </c>
       <c r="G6" t="s">
-        <v>1525</v>
+        <v>1579</v>
       </c>
       <c r="H6">
         <v>0.3779644730092272</v>
@@ -56034,13 +56196,13 @@
         <v>1459</v>
       </c>
       <c r="E7" t="s">
-        <v>1466</v>
+        <v>1471</v>
       </c>
       <c r="F7" t="s">
-        <v>1470</v>
+        <v>1524</v>
       </c>
       <c r="G7" t="s">
-        <v>1526</v>
+        <v>1580</v>
       </c>
       <c r="H7">
         <v>0.25</v>
@@ -56069,13 +56231,13 @@
         <v>1459</v>
       </c>
       <c r="E8" t="s">
-        <v>1466</v>
+        <v>1472</v>
       </c>
       <c r="F8" t="s">
-        <v>1471</v>
+        <v>1525</v>
       </c>
       <c r="G8" t="s">
-        <v>1527</v>
+        <v>1581</v>
       </c>
       <c r="H8">
         <v>0.2886751345948129</v>
@@ -56104,13 +56266,13 @@
         <v>1459</v>
       </c>
       <c r="E9" t="s">
-        <v>1466</v>
+        <v>1473</v>
       </c>
       <c r="F9" t="s">
-        <v>1472</v>
+        <v>1526</v>
       </c>
       <c r="G9" t="s">
-        <v>1527</v>
+        <v>1581</v>
       </c>
       <c r="H9">
         <v>0.2886751345948129</v>
@@ -56139,13 +56301,13 @@
         <v>1459</v>
       </c>
       <c r="E10" t="s">
-        <v>1466</v>
+        <v>1474</v>
       </c>
       <c r="F10" t="s">
-        <v>1473</v>
+        <v>1527</v>
       </c>
       <c r="G10" t="s">
-        <v>1528</v>
+        <v>1582</v>
       </c>
       <c r="H10">
         <v>0.5773502691896258</v>
@@ -56174,13 +56336,13 @@
         <v>1459</v>
       </c>
       <c r="E11" t="s">
-        <v>1466</v>
+        <v>1475</v>
       </c>
       <c r="F11" t="s">
-        <v>1474</v>
+        <v>1528</v>
       </c>
       <c r="G11" t="s">
-        <v>1527</v>
+        <v>1581</v>
       </c>
       <c r="H11">
         <v>0.2886751345948129</v>
@@ -56209,13 +56371,13 @@
         <v>1459</v>
       </c>
       <c r="E12" t="s">
-        <v>1466</v>
+        <v>1476</v>
       </c>
       <c r="F12" t="s">
-        <v>1475</v>
+        <v>1529</v>
       </c>
       <c r="G12" t="s">
-        <v>1527</v>
+        <v>1581</v>
       </c>
       <c r="H12">
         <v>0.2886751345948129</v>
@@ -56244,13 +56406,13 @@
         <v>1462</v>
       </c>
       <c r="E13" t="s">
-        <v>1466</v>
+        <v>1477</v>
       </c>
       <c r="F13" t="s">
-        <v>1476</v>
+        <v>1530</v>
       </c>
       <c r="G13" t="s">
-        <v>1529</v>
+        <v>1583</v>
       </c>
       <c r="H13">
         <v>0.2581988897471611</v>
@@ -56279,13 +56441,13 @@
         <v>1463</v>
       </c>
       <c r="E14" t="s">
-        <v>1466</v>
+        <v>1478</v>
       </c>
       <c r="F14" t="s">
-        <v>1477</v>
+        <v>1531</v>
       </c>
       <c r="G14" t="s">
-        <v>1530</v>
+        <v>1584</v>
       </c>
       <c r="H14">
         <v>0.4472135954999579</v>
@@ -56314,13 +56476,13 @@
         <v>1464</v>
       </c>
       <c r="E15" t="s">
-        <v>1466</v>
+        <v>1479</v>
       </c>
       <c r="F15" t="s">
-        <v>1478</v>
+        <v>1532</v>
       </c>
       <c r="G15" t="s">
-        <v>1527</v>
+        <v>1581</v>
       </c>
       <c r="H15">
         <v>0.2886751345948129</v>
@@ -56349,13 +56511,13 @@
         <v>1459</v>
       </c>
       <c r="E16" t="s">
-        <v>1466</v>
+        <v>1480</v>
       </c>
       <c r="F16" t="s">
-        <v>1479</v>
+        <v>1533</v>
       </c>
       <c r="G16" t="s">
-        <v>1531</v>
+        <v>1585</v>
       </c>
       <c r="H16">
         <v>0.223606797749979</v>
@@ -56384,13 +56546,13 @@
         <v>1459</v>
       </c>
       <c r="E17" t="s">
-        <v>1466</v>
+        <v>1481</v>
       </c>
       <c r="F17" t="s">
-        <v>1480</v>
+        <v>1534</v>
       </c>
       <c r="G17" t="s">
-        <v>1522</v>
+        <v>1576</v>
       </c>
       <c r="H17">
         <v>0.3162277660168379</v>
@@ -56419,13 +56581,13 @@
         <v>1459</v>
       </c>
       <c r="E18" t="s">
-        <v>1466</v>
+        <v>1482</v>
       </c>
       <c r="F18" t="s">
-        <v>1481</v>
+        <v>1535</v>
       </c>
       <c r="G18" t="s">
-        <v>1532</v>
+        <v>1586</v>
       </c>
       <c r="H18">
         <v>0.2672612419124244</v>
@@ -56454,13 +56616,13 @@
         <v>1459</v>
       </c>
       <c r="E19" t="s">
-        <v>1466</v>
+        <v>1483</v>
       </c>
       <c r="F19" t="s">
-        <v>1482</v>
+        <v>1536</v>
       </c>
       <c r="G19" t="s">
-        <v>1524</v>
+        <v>1578</v>
       </c>
       <c r="H19">
         <v>0.3015113445777636</v>
@@ -56489,13 +56651,13 @@
         <v>1459</v>
       </c>
       <c r="E20" t="s">
-        <v>1466</v>
+        <v>1484</v>
       </c>
       <c r="F20" t="s">
-        <v>1483</v>
+        <v>1537</v>
       </c>
       <c r="G20" t="s">
-        <v>1533</v>
+        <v>1587</v>
       </c>
       <c r="H20">
         <v>0.1889822365046136</v>
@@ -56524,13 +56686,13 @@
         <v>1457</v>
       </c>
       <c r="E21" t="s">
-        <v>1466</v>
+        <v>1485</v>
       </c>
       <c r="F21" t="s">
         <v>1449</v>
       </c>
       <c r="G21" t="s">
-        <v>1523</v>
+        <v>1577</v>
       </c>
       <c r="H21">
         <v>0.242535625036333</v>
@@ -56559,13 +56721,13 @@
         <v>1459</v>
       </c>
       <c r="E22" t="s">
-        <v>1466</v>
+        <v>1486</v>
       </c>
       <c r="F22" t="s">
-        <v>1484</v>
+        <v>1538</v>
       </c>
       <c r="G22" t="s">
-        <v>1525</v>
+        <v>1579</v>
       </c>
       <c r="H22">
         <v>0.3779644730092272</v>
@@ -56594,13 +56756,13 @@
         <v>1457</v>
       </c>
       <c r="E23" t="s">
-        <v>1466</v>
+        <v>1487</v>
       </c>
       <c r="F23" t="s">
-        <v>1485</v>
+        <v>1539</v>
       </c>
       <c r="G23" t="s">
-        <v>1530</v>
+        <v>1584</v>
       </c>
       <c r="H23">
         <v>0.4472135954999579</v>
@@ -56629,13 +56791,13 @@
         <v>1459</v>
       </c>
       <c r="E24" t="s">
-        <v>1466</v>
+        <v>1488</v>
       </c>
       <c r="F24" t="s">
-        <v>1486</v>
+        <v>1540</v>
       </c>
       <c r="G24" t="s">
-        <v>1524</v>
+        <v>1578</v>
       </c>
       <c r="H24">
         <v>0.3015113445777636</v>
@@ -56664,13 +56826,13 @@
         <v>1459</v>
       </c>
       <c r="E25" t="s">
-        <v>1466</v>
+        <v>1489</v>
       </c>
       <c r="F25" t="s">
-        <v>1487</v>
+        <v>1541</v>
       </c>
       <c r="G25" t="s">
-        <v>1534</v>
+        <v>1588</v>
       </c>
       <c r="H25">
         <v>0.5</v>
@@ -56699,13 +56861,13 @@
         <v>1459</v>
       </c>
       <c r="E26" t="s">
-        <v>1466</v>
+        <v>1490</v>
       </c>
       <c r="F26" t="s">
-        <v>1488</v>
+        <v>1542</v>
       </c>
       <c r="G26" t="s">
-        <v>1527</v>
+        <v>1581</v>
       </c>
       <c r="H26">
         <v>0.2886751345948129</v>
@@ -56734,13 +56896,13 @@
         <v>1459</v>
       </c>
       <c r="E27" t="s">
-        <v>1466</v>
+        <v>1490</v>
       </c>
       <c r="F27" t="s">
-        <v>1489</v>
+        <v>1543</v>
       </c>
       <c r="G27" t="s">
-        <v>1535</v>
+        <v>1589</v>
       </c>
       <c r="H27">
         <v>0.7071067811865475</v>
@@ -56769,13 +56931,13 @@
         <v>1459</v>
       </c>
       <c r="E28" t="s">
-        <v>1466</v>
+        <v>1491</v>
       </c>
       <c r="F28" t="s">
-        <v>1490</v>
+        <v>1544</v>
       </c>
       <c r="G28" t="s">
-        <v>1536</v>
+        <v>1590</v>
       </c>
       <c r="H28">
         <v>0.4082482904638631</v>
@@ -56804,13 +56966,13 @@
         <v>1459</v>
       </c>
       <c r="E29" t="s">
-        <v>1466</v>
+        <v>1492</v>
       </c>
       <c r="F29" t="s">
-        <v>1491</v>
+        <v>1545</v>
       </c>
       <c r="G29" t="s">
-        <v>1536</v>
+        <v>1590</v>
       </c>
       <c r="H29">
         <v>0.4082482904638631</v>
@@ -56839,13 +57001,13 @@
         <v>1460</v>
       </c>
       <c r="E30" t="s">
-        <v>1466</v>
+        <v>1493</v>
       </c>
       <c r="F30" t="s">
-        <v>1492</v>
+        <v>1546</v>
       </c>
       <c r="G30" t="s">
-        <v>1524</v>
+        <v>1578</v>
       </c>
       <c r="H30">
         <v>0.3015113445777636</v>
@@ -56874,13 +57036,13 @@
         <v>1462</v>
       </c>
       <c r="E31" t="s">
-        <v>1466</v>
+        <v>1494</v>
       </c>
       <c r="F31" t="s">
-        <v>1493</v>
+        <v>1547</v>
       </c>
       <c r="G31" t="s">
-        <v>1528</v>
+        <v>1582</v>
       </c>
       <c r="H31">
         <v>0.5773502691896258</v>
@@ -56909,13 +57071,13 @@
         <v>1459</v>
       </c>
       <c r="E32" t="s">
-        <v>1466</v>
+        <v>1495</v>
       </c>
       <c r="F32" t="s">
-        <v>1494</v>
+        <v>1548</v>
       </c>
       <c r="G32" t="s">
-        <v>1527</v>
+        <v>1581</v>
       </c>
       <c r="H32">
         <v>0.2886751345948129</v>
@@ -56944,13 +57106,13 @@
         <v>1459</v>
       </c>
       <c r="E33" t="s">
-        <v>1466</v>
+        <v>1496</v>
       </c>
       <c r="F33" t="s">
-        <v>1495</v>
+        <v>1549</v>
       </c>
       <c r="G33" t="s">
-        <v>1537</v>
+        <v>1591</v>
       </c>
       <c r="H33">
         <v>0.2357022603955159</v>
@@ -56979,13 +57141,13 @@
         <v>1459</v>
       </c>
       <c r="E34" t="s">
-        <v>1466</v>
+        <v>1497</v>
       </c>
       <c r="F34" t="s">
-        <v>1496</v>
+        <v>1550</v>
       </c>
       <c r="G34" t="s">
-        <v>1524</v>
+        <v>1578</v>
       </c>
       <c r="H34">
         <v>0.3015113445777636</v>
@@ -57014,13 +57176,13 @@
         <v>1459</v>
       </c>
       <c r="E35" t="s">
-        <v>1466</v>
+        <v>1498</v>
       </c>
       <c r="F35" t="s">
         <v>1449</v>
       </c>
       <c r="G35" t="s">
-        <v>1536</v>
+        <v>1590</v>
       </c>
       <c r="H35">
         <v>0.4082482904638631</v>
@@ -57049,13 +57211,13 @@
         <v>1465</v>
       </c>
       <c r="E36" t="s">
-        <v>1466</v>
+        <v>1499</v>
       </c>
       <c r="F36" t="s">
-        <v>1497</v>
+        <v>1551</v>
       </c>
       <c r="G36" t="s">
-        <v>1536</v>
+        <v>1590</v>
       </c>
       <c r="H36">
         <v>0.4082482904638631</v>
@@ -57084,13 +57246,13 @@
         <v>1459</v>
       </c>
       <c r="E37" t="s">
-        <v>1466</v>
+        <v>1500</v>
       </c>
       <c r="F37" t="s">
-        <v>1498</v>
+        <v>1552</v>
       </c>
       <c r="G37" t="s">
-        <v>1532</v>
+        <v>1586</v>
       </c>
       <c r="H37">
         <v>0.2672612419124244</v>
@@ -57119,13 +57281,13 @@
         <v>1459</v>
       </c>
       <c r="E38" t="s">
-        <v>1466</v>
+        <v>1501</v>
       </c>
       <c r="F38" t="s">
-        <v>1499</v>
+        <v>1553</v>
       </c>
       <c r="G38" t="s">
-        <v>1529</v>
+        <v>1583</v>
       </c>
       <c r="H38">
         <v>0.2581988897471611</v>
@@ -57154,13 +57316,13 @@
         <v>1459</v>
       </c>
       <c r="E39" t="s">
-        <v>1466</v>
+        <v>1502</v>
       </c>
       <c r="F39" t="s">
-        <v>1500</v>
+        <v>1554</v>
       </c>
       <c r="G39" t="s">
-        <v>1538</v>
+        <v>1592</v>
       </c>
       <c r="H39">
         <v>0.3535533905932737</v>
@@ -57189,13 +57351,13 @@
         <v>1459</v>
       </c>
       <c r="E40" t="s">
-        <v>1466</v>
+        <v>1497</v>
       </c>
       <c r="F40" t="s">
-        <v>1501</v>
+        <v>1555</v>
       </c>
       <c r="G40" t="s">
-        <v>1538</v>
+        <v>1592</v>
       </c>
       <c r="H40">
         <v>0.3535533905932737</v>
@@ -57224,13 +57386,13 @@
         <v>1460</v>
       </c>
       <c r="E41" t="s">
-        <v>1466</v>
+        <v>1503</v>
       </c>
       <c r="F41" t="s">
-        <v>1502</v>
+        <v>1556</v>
       </c>
       <c r="G41" t="s">
-        <v>1538</v>
+        <v>1592</v>
       </c>
       <c r="H41">
         <v>0.3535533905932737</v>
@@ -57259,13 +57421,13 @@
         <v>1459</v>
       </c>
       <c r="E42" t="s">
-        <v>1466</v>
+        <v>1504</v>
       </c>
       <c r="F42" t="s">
-        <v>1503</v>
+        <v>1557</v>
       </c>
       <c r="G42" t="s">
-        <v>1539</v>
+        <v>1593</v>
       </c>
       <c r="H42">
         <v>0.3333333333333333</v>
@@ -57294,13 +57456,13 @@
         <v>1459</v>
       </c>
       <c r="E43" t="s">
-        <v>1466</v>
+        <v>1505</v>
       </c>
       <c r="F43" t="s">
-        <v>1504</v>
+        <v>1558</v>
       </c>
       <c r="G43" t="s">
-        <v>1522</v>
+        <v>1576</v>
       </c>
       <c r="H43">
         <v>0.3162277660168379</v>
@@ -57329,13 +57491,13 @@
         <v>1459</v>
       </c>
       <c r="E44" t="s">
-        <v>1466</v>
+        <v>1490</v>
       </c>
       <c r="F44" t="s">
-        <v>1505</v>
+        <v>1559</v>
       </c>
       <c r="G44" t="s">
-        <v>1524</v>
+        <v>1578</v>
       </c>
       <c r="H44">
         <v>0.3015113445777636</v>
@@ -57364,13 +57526,13 @@
         <v>1459</v>
       </c>
       <c r="E45" t="s">
-        <v>1466</v>
+        <v>1506</v>
       </c>
       <c r="F45" t="s">
-        <v>1506</v>
+        <v>1560</v>
       </c>
       <c r="G45" t="s">
-        <v>1524</v>
+        <v>1578</v>
       </c>
       <c r="H45">
         <v>0.3015113445777636</v>
@@ -57399,13 +57561,13 @@
         <v>1459</v>
       </c>
       <c r="E46" t="s">
-        <v>1466</v>
+        <v>1507</v>
       </c>
       <c r="F46" t="s">
-        <v>1507</v>
+        <v>1561</v>
       </c>
       <c r="G46" t="s">
-        <v>1527</v>
+        <v>1581</v>
       </c>
       <c r="H46">
         <v>0.2886751345948129</v>
@@ -57434,13 +57596,13 @@
         <v>1459</v>
       </c>
       <c r="E47" t="s">
-        <v>1466</v>
+        <v>1508</v>
       </c>
       <c r="F47" t="s">
-        <v>1508</v>
+        <v>1562</v>
       </c>
       <c r="G47" t="s">
-        <v>1527</v>
+        <v>1581</v>
       </c>
       <c r="H47">
         <v>0.2886751345948129</v>
@@ -57469,13 +57631,13 @@
         <v>1459</v>
       </c>
       <c r="E48" t="s">
-        <v>1466</v>
+        <v>1509</v>
       </c>
       <c r="F48" t="s">
-        <v>1509</v>
+        <v>1563</v>
       </c>
       <c r="G48" t="s">
-        <v>1540</v>
+        <v>1594</v>
       </c>
       <c r="H48">
         <v>0.2773500981126146</v>
@@ -57504,13 +57666,13 @@
         <v>1459</v>
       </c>
       <c r="E49" t="s">
-        <v>1466</v>
+        <v>1510</v>
       </c>
       <c r="F49" t="s">
-        <v>1510</v>
+        <v>1564</v>
       </c>
       <c r="G49" t="s">
-        <v>1532</v>
+        <v>1586</v>
       </c>
       <c r="H49">
         <v>0.2672612419124244</v>
@@ -57539,13 +57701,13 @@
         <v>1459</v>
       </c>
       <c r="E50" t="s">
-        <v>1466</v>
+        <v>1511</v>
       </c>
       <c r="F50" t="s">
-        <v>1511</v>
+        <v>1565</v>
       </c>
       <c r="G50" t="s">
-        <v>1532</v>
+        <v>1586</v>
       </c>
       <c r="H50">
         <v>0.2672612419124244</v>
@@ -57574,13 +57736,13 @@
         <v>1459</v>
       </c>
       <c r="E51" t="s">
-        <v>1466</v>
+        <v>1512</v>
       </c>
       <c r="F51" t="s">
-        <v>1512</v>
+        <v>1566</v>
       </c>
       <c r="G51" t="s">
-        <v>1523</v>
+        <v>1577</v>
       </c>
       <c r="H51">
         <v>0.242535625036333</v>
@@ -57609,13 +57771,13 @@
         <v>1459</v>
       </c>
       <c r="E52" t="s">
-        <v>1466</v>
+        <v>1513</v>
       </c>
       <c r="F52" t="s">
-        <v>1513</v>
+        <v>1567</v>
       </c>
       <c r="G52" t="s">
-        <v>1525</v>
+        <v>1579</v>
       </c>
       <c r="H52">
         <v>0.3779644730092272</v>
@@ -57644,13 +57806,13 @@
         <v>1459</v>
       </c>
       <c r="E53" t="s">
-        <v>1466</v>
+        <v>1514</v>
       </c>
       <c r="F53" t="s">
-        <v>1514</v>
+        <v>1568</v>
       </c>
       <c r="G53" t="s">
-        <v>1525</v>
+        <v>1579</v>
       </c>
       <c r="H53">
         <v>0.3779644730092272</v>
@@ -57679,13 +57841,13 @@
         <v>1459</v>
       </c>
       <c r="E54" t="s">
-        <v>1466</v>
+        <v>1515</v>
       </c>
       <c r="F54" t="s">
-        <v>1515</v>
+        <v>1569</v>
       </c>
       <c r="G54" t="s">
-        <v>1538</v>
+        <v>1592</v>
       </c>
       <c r="H54">
         <v>0.3535533905932737</v>
@@ -57714,13 +57876,13 @@
         <v>1459</v>
       </c>
       <c r="E55" t="s">
-        <v>1466</v>
+        <v>1497</v>
       </c>
       <c r="F55" t="s">
-        <v>1516</v>
+        <v>1570</v>
       </c>
       <c r="G55" t="s">
-        <v>1539</v>
+        <v>1593</v>
       </c>
       <c r="H55">
         <v>0.3333333333333333</v>
@@ -57749,13 +57911,13 @@
         <v>1459</v>
       </c>
       <c r="E56" t="s">
-        <v>1466</v>
+        <v>1516</v>
       </c>
       <c r="F56" t="s">
-        <v>1517</v>
+        <v>1571</v>
       </c>
       <c r="G56" t="s">
-        <v>1522</v>
+        <v>1576</v>
       </c>
       <c r="H56">
         <v>0.3162277660168379</v>
@@ -57784,13 +57946,13 @@
         <v>1459</v>
       </c>
       <c r="E57" t="s">
-        <v>1466</v>
+        <v>1517</v>
       </c>
       <c r="F57" t="s">
-        <v>1518</v>
+        <v>1572</v>
       </c>
       <c r="G57" t="s">
-        <v>1524</v>
+        <v>1578</v>
       </c>
       <c r="H57">
         <v>0.3015113445777636</v>
@@ -57819,13 +57981,13 @@
         <v>1459</v>
       </c>
       <c r="E58" t="s">
-        <v>1466</v>
+        <v>1518</v>
       </c>
       <c r="F58" t="s">
-        <v>1519</v>
+        <v>1573</v>
       </c>
       <c r="G58" t="s">
-        <v>1532</v>
+        <v>1586</v>
       </c>
       <c r="H58">
         <v>0.2672612419124244</v>
@@ -57854,13 +58016,13 @@
         <v>1459</v>
       </c>
       <c r="E59" t="s">
-        <v>1466</v>
+        <v>1519</v>
       </c>
       <c r="F59" t="s">
-        <v>1520</v>
+        <v>1574</v>
       </c>
       <c r="G59" t="s">
-        <v>1532</v>
+        <v>1586</v>
       </c>
       <c r="H59">
         <v>0.2672612419124244</v>
@@ -57889,13 +58051,13 @@
         <v>1459</v>
       </c>
       <c r="E60" t="s">
-        <v>1466</v>
+        <v>1520</v>
       </c>
       <c r="F60" t="s">
-        <v>1521</v>
+        <v>1575</v>
       </c>
       <c r="G60" t="s">
-        <v>1532</v>
+        <v>1586</v>
       </c>
       <c r="H60">
         <v>0.2672612419124244</v>

</xml_diff>